<commit_message>
Manual corrections to TAA, MAR and LOM
</commit_message>
<xml_diff>
--- a/external/correzioni/LOM_edit.xlsx
+++ b/external/correzioni/LOM_edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidenicoli/Local_Workspace/TesiMag/external/correzioni/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286BD66D-4FA1-6C4A-8B58-C27FC480CEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECE7B5F-4ECB-3F4E-A6EF-85DCC34E3CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="14400" windowWidth="20480" windowHeight="12800" xr2:uid="{66C82EF7-C586-6446-BEFD-FAA6C937A404}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" xr2:uid="{66C82EF7-C586-6446-BEFD-FAA6C937A404}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -3095,9 +3095,6 @@
     <t>lon_ok</t>
   </si>
   <si>
-    <t>elev_ok</t>
-  </si>
-  <si>
     <t>loc_precision</t>
   </si>
   <si>
@@ -3222,6 +3219,9 @@
   </si>
   <si>
     <t>La quota non mi convince - Valuatere se correggere</t>
+  </si>
+  <si>
+    <t>ele_ok</t>
   </si>
 </sst>
 </file>
@@ -3364,6 +3364,12 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -3382,12 +3388,6 @@
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3402,7 +3402,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6A6FD721-0DF3-CC4D-8369-DE5F934858BC}" name="Tabella1" displayName="Tabella1" ref="A1:AH354" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6A6FD721-0DF3-CC4D-8369-DE5F934858BC}" name="Tabella1" displayName="Tabella1" ref="A1:AH354" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:AH354" xr:uid="{6A6FD721-0DF3-CC4D-8369-DE5F934858BC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AH354">
     <sortCondition ref="E1:E354"/>
@@ -3429,14 +3429,14 @@
     <tableColumn id="19" xr3:uid="{8CB66C82-2692-204B-B998-2904C37C71B2}" name="dataset"/>
     <tableColumn id="20" xr3:uid="{E255C6D8-DB0D-5B4F-8F55-552644A1AD8E}" name="from_sensor_keys"/>
     <tableColumn id="21" xr3:uid="{D2477E98-D2ED-6E4C-A7AE-4847A7E1FD3E}" name="from_datasets"/>
-    <tableColumn id="22" xr3:uid="{8245B968-4369-2C48-87F8-4381DCD5BE9E}" name="series_first" dataDxfId="2"/>
-    <tableColumn id="23" xr3:uid="{7AB20C7B-6230-C544-B7B4-0735D32770A9}" name="series_last" dataDxfId="1"/>
+    <tableColumn id="22" xr3:uid="{8245B968-4369-2C48-87F8-4381DCD5BE9E}" name="series_first" dataDxfId="1"/>
+    <tableColumn id="23" xr3:uid="{7AB20C7B-6230-C544-B7B4-0735D32770A9}" name="series_last" dataDxfId="0"/>
     <tableColumn id="24" xr3:uid="{2EEDBE26-EA12-BA41-ABBA-8DE712C99A79}" name="valid_days"/>
     <tableColumn id="25" xr3:uid="{7CFF2425-6965-A04C-9906-A3FDD1911CCC}" name="valid90"/>
     <tableColumn id="26" xr3:uid="{32B74F8E-7936-FC4C-90DF-2CEBC40C41A5}" name="original_dataset"/>
     <tableColumn id="27" xr3:uid="{57593430-C328-6448-9A86-F1156AD469ED}" name="lat_ok"/>
     <tableColumn id="28" xr3:uid="{2A7381A8-286A-BD42-904C-08218E2C2EEB}" name="lon_ok"/>
-    <tableColumn id="29" xr3:uid="{C7275A8F-82D1-C042-A8F5-FCECB38BB914}" name="elev_ok"/>
+    <tableColumn id="29" xr3:uid="{C7275A8F-82D1-C042-A8F5-FCECB38BB914}" name="ele_ok"/>
     <tableColumn id="30" xr3:uid="{C194E0D9-744A-7F42-8B9D-63190A04A7F9}" name="loc_precision"/>
     <tableColumn id="31" xr3:uid="{318EFF3B-491A-E94B-801C-684ED4CC5F11}" name="elev_precision"/>
     <tableColumn id="32" xr3:uid="{AE075CC3-A344-B648-97F1-B01D4F265BCD}" name="source"/>
@@ -3766,10 +3766,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85FFD31C-56AE-B342-9532-41E8E2AA60EF}">
   <dimension ref="A1:AH354"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E99" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
       <selection activeCell="E220" sqref="E220"/>
-      <selection pane="topRight" activeCell="AB110" sqref="AB110"/>
+      <selection pane="topRight" activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3890,22 +3890,22 @@
         <v>1018</v>
       </c>
       <c r="AC1" s="3" t="s">
+        <v>1061</v>
+      </c>
+      <c r="AD1" s="3" t="s">
         <v>1019</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>1020</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>1021</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>1022</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>1023</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
@@ -4085,7 +4085,7 @@
         <v>0</v>
       </c>
       <c r="AH3" s="5" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
@@ -4179,11 +4179,11 @@
       <c r="AD4" s="6"/>
       <c r="AE4" s="6"/>
       <c r="AF4" s="6" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="AG4" s="6"/>
       <c r="AH4" s="6" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
@@ -4279,7 +4279,7 @@
         <v>0</v>
       </c>
       <c r="AH5" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
@@ -4369,7 +4369,7 @@
       <c r="AF6" s="6"/>
       <c r="AG6" s="6"/>
       <c r="AH6" s="6" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
@@ -4469,7 +4469,7 @@
       <c r="AF7" s="6"/>
       <c r="AG7" s="6"/>
       <c r="AH7" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
@@ -4563,7 +4563,7 @@
       <c r="AF8" s="6"/>
       <c r="AG8" s="6"/>
       <c r="AH8" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
@@ -4745,7 +4745,7 @@
       <c r="AF10" s="6"/>
       <c r="AG10" s="6"/>
       <c r="AH10" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
@@ -4927,11 +4927,11 @@
       <c r="AD12" s="6"/>
       <c r="AE12" s="6"/>
       <c r="AF12" s="6" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="AG12" s="6"/>
       <c r="AH12" s="6" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.2">
@@ -5113,7 +5113,7 @@
       <c r="AF14" s="6"/>
       <c r="AG14" s="6"/>
       <c r="AH14" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.2">
@@ -6195,7 +6195,7 @@
         <v>0</v>
       </c>
       <c r="AH26" s="5" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.2">
@@ -7179,7 +7179,7 @@
         <v>0</v>
       </c>
       <c r="AH37" s="6" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="38" spans="1:34" x14ac:dyDescent="0.2">
@@ -7543,7 +7543,7 @@
       <c r="AF41" s="6"/>
       <c r="AG41" s="6"/>
       <c r="AH41" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.2">
@@ -8183,7 +8183,7 @@
       <c r="AF48" s="6"/>
       <c r="AG48" s="6"/>
       <c r="AH48" s="6" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="49" spans="1:34" x14ac:dyDescent="0.2">
@@ -8281,7 +8281,7 @@
       <c r="AF49" s="6"/>
       <c r="AG49" s="6"/>
       <c r="AH49" s="6" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="50" spans="1:34" x14ac:dyDescent="0.2">
@@ -9267,7 +9267,7 @@
       <c r="AF60" s="6"/>
       <c r="AG60" s="6"/>
       <c r="AH60" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="61" spans="1:34" x14ac:dyDescent="0.2">
@@ -9901,7 +9901,7 @@
       <c r="AF67" s="6"/>
       <c r="AG67" s="6"/>
       <c r="AH67" s="6" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="68" spans="1:34" x14ac:dyDescent="0.2">
@@ -9993,7 +9993,7 @@
       <c r="AF68" s="6"/>
       <c r="AG68" s="6"/>
       <c r="AH68" s="6" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="69" spans="1:34" x14ac:dyDescent="0.2">
@@ -10355,7 +10355,7 @@
       <c r="AF72" s="6"/>
       <c r="AG72" s="6"/>
       <c r="AH72" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="73" spans="1:34" x14ac:dyDescent="0.2">
@@ -10629,7 +10629,7 @@
       <c r="AF75" s="6"/>
       <c r="AG75" s="6"/>
       <c r="AH75" s="6" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="76" spans="1:34" x14ac:dyDescent="0.2">
@@ -11719,7 +11719,7 @@
         <v>0</v>
       </c>
       <c r="AH87" s="5" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="88" spans="1:34" x14ac:dyDescent="0.2">
@@ -12083,7 +12083,7 @@
         <v>0</v>
       </c>
       <c r="AH91" s="5" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="92" spans="1:34" x14ac:dyDescent="0.2">
@@ -13155,7 +13155,7 @@
       <c r="AF103" s="6"/>
       <c r="AG103" s="6"/>
       <c r="AH103" s="6" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="104" spans="1:34" x14ac:dyDescent="0.2">
@@ -14141,7 +14141,7 @@
       <c r="AF114" s="9"/>
       <c r="AG114" s="9"/>
       <c r="AH114" s="9" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="115" spans="1:34" x14ac:dyDescent="0.2">
@@ -14765,7 +14765,7 @@
       <c r="AF121" s="6"/>
       <c r="AG121" s="6"/>
       <c r="AH121" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="122" spans="1:34" x14ac:dyDescent="0.2">
@@ -15739,7 +15739,7 @@
         <v>0</v>
       </c>
       <c r="AH132" s="5" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="133" spans="1:34" x14ac:dyDescent="0.2">
@@ -16095,7 +16095,7 @@
         <v>0</v>
       </c>
       <c r="AH136" s="6" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="137" spans="1:34" x14ac:dyDescent="0.2">
@@ -16631,7 +16631,7 @@
       <c r="AF142" s="6"/>
       <c r="AG142" s="6"/>
       <c r="AH142" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="143" spans="1:34" x14ac:dyDescent="0.2">
@@ -16811,7 +16811,7 @@
       <c r="AF144" s="6"/>
       <c r="AG144" s="6"/>
       <c r="AH144" s="6" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="145" spans="1:34" x14ac:dyDescent="0.2">
@@ -16903,7 +16903,7 @@
       <c r="AF145" s="6"/>
       <c r="AG145" s="6"/>
       <c r="AH145" s="6" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="146" spans="1:34" x14ac:dyDescent="0.2">
@@ -17261,7 +17261,7 @@
         <v>0</v>
       </c>
       <c r="AH149" s="5" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="150" spans="1:34" x14ac:dyDescent="0.2">
@@ -17533,7 +17533,7 @@
       <c r="AF152" s="6"/>
       <c r="AG152" s="6"/>
       <c r="AH152" s="6" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="153" spans="1:34" x14ac:dyDescent="0.2">
@@ -17625,7 +17625,7 @@
         <v>0</v>
       </c>
       <c r="AH153" s="5" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="154" spans="1:34" x14ac:dyDescent="0.2">
@@ -17721,7 +17721,7 @@
       <c r="AF154" s="6"/>
       <c r="AG154" s="6"/>
       <c r="AH154" s="6" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="155" spans="1:34" x14ac:dyDescent="0.2">
@@ -17995,7 +17995,7 @@
       <c r="AF157" s="6"/>
       <c r="AG157" s="6"/>
       <c r="AH157" s="6" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="158" spans="1:34" x14ac:dyDescent="0.2">
@@ -19417,7 +19417,7 @@
       <c r="AF173" s="6"/>
       <c r="AG173" s="6"/>
       <c r="AH173" s="6" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="174" spans="1:34" x14ac:dyDescent="0.2">
@@ -20041,7 +20041,7 @@
       <c r="AF180" s="6"/>
       <c r="AG180" s="6"/>
       <c r="AH180" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="181" spans="1:34" x14ac:dyDescent="0.2">
@@ -20313,7 +20313,7 @@
       <c r="AF183" s="6"/>
       <c r="AG183" s="6"/>
       <c r="AH183" s="6" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="184" spans="1:34" x14ac:dyDescent="0.2">
@@ -20581,7 +20581,7 @@
         <v>0</v>
       </c>
       <c r="AH186" s="5" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="187" spans="1:34" x14ac:dyDescent="0.2">
@@ -22173,7 +22173,7 @@
       <c r="AF204" s="6"/>
       <c r="AG204" s="6"/>
       <c r="AH204" s="6" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="205" spans="1:34" x14ac:dyDescent="0.2">
@@ -22531,7 +22531,7 @@
       <c r="AF208" s="6"/>
       <c r="AG208" s="6"/>
       <c r="AH208" s="6" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="209" spans="1:34" x14ac:dyDescent="0.2">
@@ -22713,11 +22713,11 @@
       <c r="AD210" s="6"/>
       <c r="AE210" s="6"/>
       <c r="AF210" s="6" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="AG210" s="6"/>
       <c r="AH210" s="6" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="211" spans="1:34" x14ac:dyDescent="0.2">
@@ -22813,7 +22813,7 @@
       <c r="AF211" s="10"/>
       <c r="AG211" s="10"/>
       <c r="AH211" s="10" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="212" spans="1:34" x14ac:dyDescent="0.2">
@@ -25457,7 +25457,7 @@
       <c r="AF241" s="6"/>
       <c r="AG241" s="6"/>
       <c r="AH241" s="6" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="242" spans="1:34" x14ac:dyDescent="0.2">
@@ -26611,7 +26611,7 @@
       <c r="AF254" s="6"/>
       <c r="AG254" s="6"/>
       <c r="AH254" s="6" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="255" spans="1:34" x14ac:dyDescent="0.2">
@@ -27233,7 +27233,7 @@
         <v>0</v>
       </c>
       <c r="AH261" s="5" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="262" spans="1:34" x14ac:dyDescent="0.2">
@@ -27329,7 +27329,7 @@
       <c r="AF262" s="6"/>
       <c r="AG262" s="6"/>
       <c r="AH262" s="6" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="263" spans="1:34" x14ac:dyDescent="0.2">
@@ -28127,7 +28127,7 @@
         <v>0</v>
       </c>
       <c r="AH271" s="5" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="272" spans="1:34" x14ac:dyDescent="0.2">
@@ -28397,7 +28397,7 @@
         <v>0</v>
       </c>
       <c r="AH274" s="5" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="275" spans="1:34" x14ac:dyDescent="0.2">
@@ -28493,7 +28493,7 @@
       <c r="AF275" s="6"/>
       <c r="AG275" s="6"/>
       <c r="AH275" s="6" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="276" spans="1:34" x14ac:dyDescent="0.2">
@@ -28857,7 +28857,7 @@
       </c>
       <c r="AG279" s="6"/>
       <c r="AH279" s="6" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="280" spans="1:34" x14ac:dyDescent="0.2">
@@ -30189,7 +30189,7 @@
       <c r="AF294" s="6"/>
       <c r="AG294" s="6"/>
       <c r="AH294" s="6" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="295" spans="1:34" x14ac:dyDescent="0.2">
@@ -30989,7 +30989,7 @@
       <c r="AF303" s="6"/>
       <c r="AG303" s="6"/>
       <c r="AH303" s="6" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="304" spans="1:34" x14ac:dyDescent="0.2">
@@ -32049,7 +32049,7 @@
         <v>0</v>
       </c>
       <c r="AH315" s="5" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="316" spans="1:34" x14ac:dyDescent="0.2">
@@ -33023,7 +33023,7 @@
       <c r="AF326" s="7"/>
       <c r="AG326" s="7"/>
       <c r="AH326" s="7" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="327" spans="1:34" x14ac:dyDescent="0.2">
@@ -33203,7 +33203,7 @@
         <v>0</v>
       </c>
       <c r="AH328" s="5" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="329" spans="1:34" x14ac:dyDescent="0.2">
@@ -33651,7 +33651,7 @@
       <c r="AF333" s="6"/>
       <c r="AG333" s="6"/>
       <c r="AH333" s="6" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="334" spans="1:34" x14ac:dyDescent="0.2">
@@ -33747,7 +33747,7 @@
       <c r="AF334" s="6"/>
       <c r="AG334" s="6"/>
       <c r="AH334" s="6" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="335" spans="1:34" x14ac:dyDescent="0.2">
@@ -34103,7 +34103,7 @@
       <c r="AF338" s="6"/>
       <c r="AG338" s="6"/>
       <c r="AH338" s="6" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="339" spans="1:34" x14ac:dyDescent="0.2">
@@ -34199,7 +34199,7 @@
       <c r="AF339" s="6"/>
       <c r="AG339" s="6"/>
       <c r="AH339" s="6" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="340" spans="1:34" x14ac:dyDescent="0.2">
@@ -34383,7 +34383,7 @@
       <c r="AF341" s="6"/>
       <c r="AG341" s="6"/>
       <c r="AH341" s="6" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="342" spans="1:34" x14ac:dyDescent="0.2">
@@ -34835,7 +34835,7 @@
       <c r="AF346" s="6"/>
       <c r="AG346" s="6"/>
       <c r="AH346" s="6" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="347" spans="1:34" x14ac:dyDescent="0.2">

</xml_diff>